<commit_message>
Capsulation and stylization change
</commit_message>
<xml_diff>
--- a/src/main/resources/data/DomesticRotterdamDatabase.xlsx
+++ b/src/main/resources/data/DomesticRotterdamDatabase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EasyImport\src\main\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EasyImport\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F9A95A-E82C-4054-8582-FA8DCACEECCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C812530-2216-4649-BAD1-1E128E59E9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AADEE7A6-3B55-4ACB-90D7-0056688B84BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AADEE7A6-3B55-4ACB-90D7-0056688B84BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,34 +62,34 @@
     <t>POD</t>
   </si>
   <si>
-    <t>NEW YORK</t>
-  </si>
-  <si>
-    <t>SAVANNAH</t>
-  </si>
-  <si>
-    <t>HOUSTON</t>
-  </si>
-  <si>
-    <t>INDIANAPOLIS</t>
-  </si>
-  <si>
-    <t>LOS ANGELES</t>
-  </si>
-  <si>
-    <t>ROTTERDAM</t>
-  </si>
-  <si>
-    <t>VARNA</t>
-  </si>
-  <si>
     <t>MOTORCYCLE</t>
   </si>
   <si>
-    <t>MIAMI</t>
-  </si>
-  <si>
-    <t>SAN FRANCISCO</t>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Savannah</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Indianapolis</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>Rotterdam</t>
+  </si>
+  <si>
+    <t>Varna</t>
   </si>
 </sst>
 </file>
@@ -496,20 +496,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8EFC55B-AADF-4BE0-95D6-CC78F3EF7287}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -523,12 +523,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -537,12 +537,12 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -551,12 +551,12 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -565,12 +565,12 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -579,26 +579,26 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D6" s="1">
         <v>1300</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
@@ -607,12 +607,12 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
@@ -621,12 +621,12 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
@@ -635,12 +635,12 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -649,26 +649,26 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1">
         <v>1300</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1</v>
@@ -677,12 +677,12 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>2</v>
@@ -691,12 +691,12 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
@@ -705,12 +705,12 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
@@ -719,26 +719,26 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1">
         <v>1300</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1</v>
@@ -747,12 +747,12 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>2</v>
@@ -761,12 +761,12 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>3</v>
@@ -775,12 +775,12 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>4</v>
@@ -789,26 +789,26 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D21" s="1">
         <v>1300</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>1</v>
@@ -817,12 +817,12 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>2</v>
@@ -831,12 +831,12 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>3</v>
@@ -845,12 +845,12 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>4</v>
@@ -859,26 +859,26 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D26" s="1">
         <v>1300</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>1</v>
@@ -887,12 +887,12 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>2</v>
@@ -901,12 +901,12 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>3</v>
@@ -915,12 +915,12 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>4</v>
@@ -929,26 +929,26 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D31" s="1">
         <v>1300</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>1</v>
@@ -957,12 +957,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>2</v>
@@ -971,12 +971,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>3</v>
@@ -985,12 +985,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>4</v>
@@ -999,26 +999,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>1</v>
@@ -1027,12 +1027,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>2</v>
@@ -1041,12 +1041,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>3</v>
@@ -1055,12 +1055,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>4</v>
@@ -1069,26 +1069,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D41" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>1</v>
@@ -1097,12 +1097,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>2</v>
@@ -1111,12 +1111,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>3</v>
@@ -1125,12 +1125,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>4</v>
@@ -1139,26 +1139,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>1</v>
@@ -1167,12 +1167,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>2</v>
@@ -1181,12 +1181,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>3</v>
@@ -1195,12 +1195,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>4</v>
@@ -1209,26 +1209,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>1</v>
@@ -1237,12 +1237,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>2</v>
@@ -1251,12 +1251,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>3</v>
@@ -1265,12 +1265,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>4</v>
@@ -1279,26 +1279,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>1</v>
@@ -1307,12 +1307,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>2</v>
@@ -1321,12 +1321,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>3</v>
@@ -1335,12 +1335,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>4</v>
@@ -1349,26 +1349,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D61" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="B62" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>1</v>
@@ -1377,12 +1377,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>2</v>
@@ -1391,12 +1391,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>3</v>
@@ -1405,12 +1405,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>4</v>
@@ -1419,26 +1419,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D66" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="B67" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>1</v>
@@ -1447,12 +1447,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>2</v>
@@ -1461,12 +1461,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>3</v>
@@ -1475,12 +1475,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>4</v>
@@ -1489,15 +1489,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D71" s="1">
         <v>0</v>

</xml_diff>